<commit_message>
canopy running time update
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\process mining\pm4py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3537EBCB-0846-4F43-9EAB-923F2C9114C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC4BC8E-16BE-4091-80C8-8D9A71DCB5C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C1753F0F-FFC1-467F-9ECD-AF02EB500D34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C1753F0F-FFC1-467F-9ECD-AF02EB500D34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="73">
   <si>
     <t>total 819</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,6 +286,18 @@
   </si>
   <si>
     <t>cluster 6</t>
+  </si>
+  <si>
+    <t>k means</t>
+  </si>
+  <si>
+    <t>canopy</t>
+  </si>
+  <si>
+    <t>2w</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
@@ -658,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8B2EC-DD97-4072-9002-9DD13F52F6A9}">
   <dimension ref="A5:AA324"/>
   <sheetViews>
-    <sheetView topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="V318" sqref="V318"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -749,6 +761,15 @@
       </c>
     </row>
     <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <v>1690.47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
@@ -779,6 +800,15 @@
       </c>
     </row>
     <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>13.962999999999999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -2117,6 +2147,15 @@
       </c>
     </row>
     <row r="51" spans="1:27">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51">
+        <v>23797.365000000002</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
       <c r="E51" t="s">
         <v>13</v>
       </c>
@@ -2147,6 +2186,15 @@
       </c>
     </row>
     <row r="52" spans="1:27">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52">
+        <v>4290.3220000000001</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
       <c r="D52" t="s">
         <v>14</v>
       </c>
@@ -3482,6 +3530,15 @@
       </c>
     </row>
     <row r="96" spans="1:27">
+      <c r="A96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96">
+        <v>40449.991000000002</v>
+      </c>
+      <c r="C96" t="s">
+        <v>72</v>
+      </c>
       <c r="E96" t="s">
         <v>13</v>
       </c>
@@ -3511,7 +3568,16 @@
         <v>0.520696512</v>
       </c>
     </row>
-    <row r="97" spans="4:27">
+    <row r="97" spans="1:27">
+      <c r="A97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97">
+        <v>43845.118999999999</v>
+      </c>
+      <c r="C97" t="s">
+        <v>72</v>
+      </c>
       <c r="D97" t="s">
         <v>14</v>
       </c>
@@ -3552,7 +3618,10 @@
         <v>0.44078836799999999</v>
       </c>
     </row>
-    <row r="98" spans="4:27">
+    <row r="98" spans="1:27">
+      <c r="A98" t="s">
+        <v>71</v>
+      </c>
       <c r="E98" t="s">
         <v>13</v>
       </c>
@@ -3582,7 +3651,7 @@
         <v>0.25553999999999999</v>
       </c>
     </row>
-    <row r="99" spans="4:27">
+    <row r="99" spans="1:27">
       <c r="E99" t="s">
         <v>15</v>
       </c>
@@ -3612,7 +3681,7 @@
         <v>6.5122200000000005E-2</v>
       </c>
     </row>
-    <row r="100" spans="4:27">
+    <row r="100" spans="1:27">
       <c r="D100" t="s">
         <v>16</v>
       </c>
@@ -3653,7 +3722,7 @@
         <v>0.40280608200000001</v>
       </c>
     </row>
-    <row r="101" spans="4:27">
+    <row r="101" spans="1:27">
       <c r="E101" t="s">
         <v>17</v>
       </c>
@@ -3683,7 +3752,7 @@
         <v>0.24494250000000001</v>
       </c>
     </row>
-    <row r="102" spans="4:27">
+    <row r="102" spans="1:27">
       <c r="E102" t="s">
         <v>18</v>
       </c>
@@ -3713,7 +3782,7 @@
         <v>3.4945393999999998E-2</v>
       </c>
     </row>
-    <row r="103" spans="4:27">
+    <row r="103" spans="1:27">
       <c r="E103" t="s">
         <v>19</v>
       </c>
@@ -3743,7 +3812,7 @@
         <v>0.12012616799999999</v>
       </c>
     </row>
-    <row r="104" spans="4:27">
+    <row r="104" spans="1:27">
       <c r="D104" t="s">
         <v>43</v>
       </c>
@@ -3751,27 +3820,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="4:27">
+    <row r="105" spans="1:27">
       <c r="E105" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="4:27">
+    <row r="106" spans="1:27">
       <c r="E106" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="4:27">
+    <row r="107" spans="1:27">
       <c r="E107" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="4:27">
+    <row r="108" spans="1:27">
       <c r="E108" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="4:27">
+    <row r="109" spans="1:27">
       <c r="D109" t="s">
         <v>49</v>
       </c>
@@ -3779,17 +3848,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="4:27">
+    <row r="110" spans="1:27">
       <c r="E110" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="4:27">
+    <row r="111" spans="1:27">
       <c r="E111" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="4:27">
+    <row r="112" spans="1:27">
       <c r="E112" t="s">
         <v>19</v>
       </c>
@@ -4271,6 +4340,15 @@
       </c>
     </row>
     <row r="138" spans="1:27">
+      <c r="A138" t="s">
+        <v>69</v>
+      </c>
+      <c r="B138">
+        <v>57653.091999999997</v>
+      </c>
+      <c r="C138" t="s">
+        <v>72</v>
+      </c>
       <c r="E138" t="s">
         <v>17</v>
       </c>
@@ -4301,6 +4379,15 @@
       </c>
     </row>
     <row r="139" spans="1:27">
+      <c r="A139" t="s">
+        <v>70</v>
+      </c>
+      <c r="B139">
+        <v>11309.031000000001</v>
+      </c>
+      <c r="C139" t="s">
+        <v>72</v>
+      </c>
       <c r="D139" t="s">
         <v>33</v>
       </c>
@@ -4342,6 +4429,9 @@
       </c>
     </row>
     <row r="140" spans="1:27">
+      <c r="A140" t="s">
+        <v>71</v>
+      </c>
       <c r="E140" t="s">
         <v>17</v>
       </c>
@@ -5643,6 +5733,15 @@
       </c>
     </row>
     <row r="182" spans="1:27">
+      <c r="A182" t="s">
+        <v>69</v>
+      </c>
+      <c r="B182">
+        <v>1915.4169999999999</v>
+      </c>
+      <c r="C182" t="s">
+        <v>72</v>
+      </c>
       <c r="E182" t="s">
         <v>13</v>
       </c>
@@ -5673,6 +5772,15 @@
       </c>
     </row>
     <row r="183" spans="1:27">
+      <c r="A183" t="s">
+        <v>70</v>
+      </c>
+      <c r="B183">
+        <v>4610.7049999999999</v>
+      </c>
+      <c r="C183" t="s">
+        <v>72</v>
+      </c>
       <c r="D183" t="s">
         <v>14</v>
       </c>
@@ -6422,6 +6530,15 @@
       </c>
     </row>
     <row r="227" spans="1:27">
+      <c r="A227" t="s">
+        <v>69</v>
+      </c>
+      <c r="B227">
+        <v>61366.180999999997</v>
+      </c>
+      <c r="C227" t="s">
+        <v>72</v>
+      </c>
       <c r="E227" t="s">
         <v>13</v>
       </c>
@@ -6452,6 +6569,15 @@
       </c>
     </row>
     <row r="228" spans="1:27">
+      <c r="A228" t="s">
+        <v>70</v>
+      </c>
+      <c r="B228">
+        <v>3858.7979999999998</v>
+      </c>
+      <c r="C228" t="s">
+        <v>72</v>
+      </c>
       <c r="D228" t="s">
         <v>52</v>
       </c>
@@ -7376,6 +7502,15 @@
       </c>
     </row>
     <row r="270" spans="1:27">
+      <c r="A270" t="s">
+        <v>69</v>
+      </c>
+      <c r="B270">
+        <v>36516.271000000001</v>
+      </c>
+      <c r="C270" t="s">
+        <v>72</v>
+      </c>
       <c r="E270" t="s">
         <v>13</v>
       </c>
@@ -7405,6 +7540,15 @@
       </c>
     </row>
     <row r="271" spans="1:27">
+      <c r="A271" t="s">
+        <v>70</v>
+      </c>
+      <c r="B271">
+        <v>15909.343999999999</v>
+      </c>
+      <c r="C271" t="s">
+        <v>72</v>
+      </c>
       <c r="D271" t="s">
         <v>14</v>
       </c>
@@ -7448,6 +7592,9 @@
       </c>
     </row>
     <row r="272" spans="1:27">
+      <c r="A272" t="s">
+        <v>71</v>
+      </c>
       <c r="E272" t="s">
         <v>13</v>
       </c>
@@ -9111,7 +9258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C590C6-CA1C-4B64-9D6E-A4DF9D9B5E9A}">
   <dimension ref="A3:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -10560,7 +10707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DDBB17-CB62-4571-9413-7E9D83057C37}">
   <dimension ref="B8:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>

</xml_diff>